<commit_message>
PCB v2.0 40mm x 40mm done
</commit_message>
<xml_diff>
--- a/TinySays_BOM.xlsx
+++ b/TinySays_BOM.xlsx
@@ -872,24 +872,19 @@
   <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="18" min="14" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="24" min="20" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="27" min="26" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>